<commit_message>
fixed "apply filter" doesn't work error in Stefan filter
</commit_message>
<xml_diff>
--- a/R/data/description_bv.xlsx
+++ b/R/data/description_bv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://abacusbio-my.sharepoint.com/personal/lzhang_abacusbio_co_nz/Documents/GitHub/test_pca/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lzhang\GitHub\index_aggregation_app\R\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4CBCF084-7214-4B1D-8A12-CF2DF087D7D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ACBDB09-D61C-4A6F-83FA-D888FF839A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="1125" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="5880" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,48 +36,6 @@
     <t>sex</t>
   </si>
   <si>
-    <t>LDSR_CERCZM_BLUP</t>
-  </si>
-  <si>
-    <t>SRSR_COLLGR_BLUP</t>
-  </si>
-  <si>
-    <t>LDSR_CORBNE_BLUP</t>
-  </si>
-  <si>
-    <t>ERSR_GIBBFU_BLUP</t>
-  </si>
-  <si>
-    <t>ERSR_GIBBZE_BLUP</t>
-  </si>
-  <si>
-    <t>LDSR_NLBR1_BLUP</t>
-  </si>
-  <si>
-    <t>LDSR_PUCCPY_BLUP</t>
-  </si>
-  <si>
-    <t>LDSR_TARSC_BLUP</t>
-  </si>
-  <si>
-    <t>YLD_BE_BLUP</t>
-  </si>
-  <si>
-    <t>AGSPP_BLUP</t>
-  </si>
-  <si>
-    <t>RTLP_BLUP</t>
-  </si>
-  <si>
-    <t>STLP_BLUP</t>
-  </si>
-  <si>
-    <t>TWT_BE_BLUP</t>
-  </si>
-  <si>
-    <t>MST_BE_BLUP</t>
-  </si>
-  <si>
     <t>classifier</t>
   </si>
   <si>
@@ -85,6 +43,48 @@
   </si>
   <si>
     <t>EBV</t>
+  </si>
+  <si>
+    <t>GLEAFSPOT</t>
+  </si>
+  <si>
+    <t>ANTHRAC</t>
+  </si>
+  <si>
+    <t>GOSSWILT</t>
+  </si>
+  <si>
+    <t>FUSARIUM</t>
+  </si>
+  <si>
+    <t>GIBBERELLA</t>
+  </si>
+  <si>
+    <t>NLEAFBLIGHT</t>
+  </si>
+  <si>
+    <t>BROWNRUST</t>
+  </si>
+  <si>
+    <t>TARSPOT</t>
+  </si>
+  <si>
+    <t>YIELD</t>
+  </si>
+  <si>
+    <t>GREENSNAP</t>
+  </si>
+  <si>
+    <t>ROOTLODGE</t>
+  </si>
+  <si>
+    <t>STALKLODGE</t>
+  </si>
+  <si>
+    <t>TESTWT</t>
+  </si>
+  <si>
+    <t>MOIST</t>
   </si>
 </sst>
 </file>
@@ -120,8 +120,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,7 +406,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,7 +419,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -434,119 +435,119 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>